<commit_message>
Refactored, redesigned - becomes more data oritented Cleared
</commit_message>
<xml_diff>
--- a/tests/resources/files/testXLSX.xlsx
+++ b/tests/resources/files/testXLSX.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="150" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="150" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="25">
   <si>
     <t>CAT - WET</t>
   </si>
@@ -47,28 +48,28 @@
 inkl. MwSt</t>
   </si>
   <si>
-    <t>Hühnerschenkel </t>
+    <t>Hühnerschenkel</t>
   </si>
   <si>
     <t>55 g</t>
   </si>
   <si>
-    <t>Hühnerbrust </t>
-  </si>
-  <si>
-    <t>Makrele </t>
-  </si>
-  <si>
-    <t>Skip Jack Thunfischfilet </t>
-  </si>
-  <si>
-    <t>Tonggol Thunfischfilet </t>
+    <t>Hühnerbrust</t>
+  </si>
+  <si>
+    <t>Makrele</t>
+  </si>
+  <si>
+    <t>Skip Jack Thunfischfilet</t>
+  </si>
+  <si>
+    <t>Tonggol Thunfischfilet</t>
   </si>
   <si>
     <t>Hühnerbrust und Entenfilet</t>
   </si>
   <si>
-    <t>Hühnerfilet mit Schinken </t>
+    <t>Hühnerfilet mit Schinken</t>
   </si>
   <si>
     <t>Hühnerfilet und Thunfischfilet</t>
@@ -77,22 +78,19 @@
     <t>GREEN LABEL</t>
   </si>
   <si>
-    <t>Hühnerfilet und Garnelen </t>
-  </si>
-  <si>
-    <t>Thunfischfilet + Hühnerfilet mit Schinken </t>
-  </si>
-  <si>
-    <t>Thunfischfilet mit Babysardinen </t>
-  </si>
-  <si>
-    <t>Pangasiusfilet </t>
-  </si>
-  <si>
-    <t>Thunfischfilet und Garnelen </t>
-  </si>
-  <si>
-    <t> </t>
+    <t>Hühnerfilet und Garnelen</t>
+  </si>
+  <si>
+    <t>Thunfischfilet + Hühnerfilet mit Schinken</t>
+  </si>
+  <si>
+    <t>Thunfischfilet mit Babysardinen</t>
+  </si>
+  <si>
+    <t>Pangasiusfilet</t>
+  </si>
+  <si>
+    <t>Thunfischfilet und Garnelen</t>
   </si>
   <si>
     <t>Lachs</t>
@@ -108,11 +106,12 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="00000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -128,12 +127,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -247,7 +240,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -257,75 +250,75 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -337,7 +330,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -409,8 +402,8 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="A1:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -555,7 +548,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="n">
         <v>8001154123227</v>
       </c>
@@ -792,9 +785,7 @@
       <c r="C17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="13" t="s">
-        <v>24</v>
-      </c>
+      <c r="D17" s="13"/>
       <c r="E17" s="11" t="s">
         <v>10</v>
       </c>
@@ -816,11 +807,9 @@
         <v>4033</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>24</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D18" s="13"/>
       <c r="E18" s="11" t="s">
         <v>10</v>
       </c>
@@ -847,4 +836,267 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="10" t="n">
+        <v>8001154123180</v>
+      </c>
+      <c r="B3" s="11" t="n">
+        <v>4200</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="H3" s="14" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I3" s="14" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="n">
+        <v>8001154123197</v>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>4201</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="H4" s="14" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I4" s="14" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="n">
+        <v>8001154123203</v>
+      </c>
+      <c r="B5" s="11" t="n">
+        <v>4202</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="H5" s="14" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I5" s="14" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="n">
+        <v>8001154123210</v>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>4203</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="H6" s="14" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I6" s="14" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="n">
+        <v>8001154123227</v>
+      </c>
+      <c r="B7" s="11" t="n">
+        <v>4204</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="H7" s="14" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I7" s="14" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="n">
+        <v>8001154123241</v>
+      </c>
+      <c r="B8" s="11" t="n">
+        <v>4205</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="H8" s="14" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I8" s="14" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="n">
+        <v>8001154124620</v>
+      </c>
+      <c r="B9" s="11" t="n">
+        <v>4206</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="H9" s="14" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I9" s="14" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="n">
+        <v>8001154124637</v>
+      </c>
+      <c r="B10" s="11" t="n">
+        <v>4207</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="H10" s="14" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I10" s="14" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>